<commit_message>
adding content col back into Marks csv and removing unused rows from Matts
</commit_message>
<xml_diff>
--- a/data/gold_standard_labeled_mickey.xlsx
+++ b/data/gold_standard_labeled_mickey.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mickey\Documents\School\MADS Courses\Milestone_3\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{15931F99-F729-4E62-8A5F-CDBFA0F97CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D717C1A9-5980-466C-BF08-1027A7819AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28695" yWindow="0" windowWidth="29010" windowHeight="15585" xr2:uid="{07758D14-9A33-47D7-897C-E21F4B6E0172}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="20475" windowHeight="11295" xr2:uid="{07758D14-9A33-47D7-897C-E21F4B6E0172}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="363">
   <si>
     <t>uuid</t>
   </si>
@@ -2078,6 +2078,38 @@
 While the roller derby team appears to have abandoned its trademark, the Bryant Street Sports LLC of New York filed for trademarks protections for “Cleveland Guardians” in 2020. The Indians objected to the application this month, and the filing was withdrawn on July 21 — which may signify the sides worked something out, or that the baseball team filed its own application.
 That would just leave the URL — with an unknown ownership calendar with the roller derby team having first right of renewal — and social media handles to be worked out.
 The Indians don’t plan to make the Guardians switch until after the 2021 season, so there’s some time to work things out, though with the team five games out of an AL wild-card spot with 65 games left in the regular season, there may not a whole lot of it left.</t>
+  </si>
+  <si>
+    <t>831880056018758842</t>
+  </si>
+  <si>
+    <t>https://www.reuters.com/article/us-china-pets-idUSKBN0OJ2TT20150603</t>
+  </si>
+  <si>
+    <t>2015-06-03</t>
+  </si>
+  <si>
+    <t>HONG KONG/SHANGHAI (Reuters) - Shanghai bank employee Frances Chen spends about a fifth of her monthly salary on her poodle Cookie, one of the millions of pet owners turning China’s pet care industry into one of the fastest growing in the world.
+A woman takes a picture with her pet dog at a shopping mall in Beijing, in this November 25, 2014 file photo. REUTERS/Kim Kyung-Hoon/Files
+Chen takes Cookie to a groomer for a weekly shower and feeds it imported food, costing her some 2,000 yuan ($320) a month. “I want to give him the best,” said the single, 26-year-old who lives with her parents. “He’s our kid. The only difference is that he can’t speak human languages.”
+Once banned by Communist leader Chairman Mao Zedong as a bourgeois pastime, having a pet has now become a symbol of financial success in China, where consultants Euromonitor forecast the pet care sector to grow by more than half to 15.8 billion yuan ($2.6 billion) by 2019, outpacing the world’s biggest market the United States, which is expected to grow just over 4 percent this year to $60.6 billion.
+The prospects have multinationals such as Mars Inc, Nestle S.A., Procter &amp; Gamble Co and Colgate-Palmolive Co licking their lips, especially as growth in the overall retail market slows along with the world’s second largest economy.
+Dogs are by far the most popular pets and dog food sales alone are expected to almost treble to over $760 million by 2019, Euromonitor data shows, as higher disposable incomes make keeping a pet an affordable luxury for more Chinese, particularly in more developed cities.
+The loneliness and stress endemic to city life are also driving the pet ownership boom: last year, some 30 million households, or nearly 7 percent of the nationwide total, owned a dog, Euromonitor said.
+Matthias Berninger, Mars global head of public affairs, said there was plenty of room for growth in China’s pet food market, which was already expanding beyond most industry expectations.
+“Pet food penetration in China is very, very low,” he told Reuters. “People didn’t believe chocolate would ever be something Chinese consumers would like, let alone that Chinese consumers would become passionate pet owners.”
+The U.S. firm renowned for its confectionery owns pet food brands including Pedigree and Whiskas.
+Mars was the market leader in China two years ago with a two-thirds share, according to the latest Euromonitor data. Nestle-owned brands were second with just over 16 percent followed by local firm Nory Pet (Shanghai) Co Ltd with an almost 7 percent share.
+“There is huge demand for pet food as owners give up feeding their dog rice and meat and switch to proper pet food,” Chen Xiuqiang, sales manager at pet food importer and distributor Guangzhou Mudi Trading Co Ltd told Reuters.
+THE CAT’S MEOW
+In addition to branded food, more Chinese are paying top yuan for pedigree dog breeds such as Tibetan mastiffs, and the services and accessories they think these prized pets deserve.
+“In big cities like Shanghai, many people feel lonely and treat pets like family,” said pet groomer Zhao Huanhuan. “People are now willing to spend on their pets as much as they are willing to spend on their parents.”
+Beijing pet photographer Yipets offers clients packages - including pet costumes and styling - that range from 388 yuan to 8,888 yuan ($63-$1,430) while a one-month dog training course at JinJiaJun Kennel can cost 5,000 yuan.
+Luxury retailers are also benefiting. U.S. firm Chrome Bones, which opened its first China franchise in Shanghai in September, said sales have risen by up to 40 percent a month.
+The brand specializes in Swarovski-crystal encrusted pet collars that cost some $260, snakeskin carriers that start at $3,800 and patent leather beds and bowls.
+“The prospects are very good,” said shop owner Chen Yinfeng.
+Pet pampering has also become big business. Cole Zhang, who owns Blue Bone near Shanghai’s Bund, offers to chauffeur canine clients in a Ferarri or a Maserati, a service he said costs up to 500 yuan a kilometer and is often booked out.
+“On average, we have more than 100 clients a week. We usually work overtime on weekends,” he added. “Most of my customers treat their dogs very well and they are willing to spend a lot on their dogs.”</t>
   </si>
 </sst>
 </file>
@@ -2504,10 +2536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68AEF014-663C-47C5-BC0A-17F67B5DB296}">
-  <dimension ref="A1:U84"/>
+  <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4001,87 +4033,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>160</v>
-      </c>
-      <c r="B34" s="2"/>
+        <v>359</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1</v>
+      </c>
       <c r="C34" s="2"/>
-      <c r="D34" s="2">
-        <v>1</v>
-      </c>
+      <c r="D34" s="2"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
+      <c r="K34" s="2">
+        <v>1</v>
+      </c>
       <c r="L34" s="2">
         <v>1</v>
       </c>
-      <c r="M34" s="2">
-        <v>1</v>
-      </c>
-      <c r="N34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2">
+        <v>1</v>
+      </c>
       <c r="O34" s="2"/>
       <c r="P34" t="s">
-        <v>161</v>
+        <v>360</v>
       </c>
       <c r="Q34" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="R34" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="S34" t="s">
-        <v>162</v>
-      </c>
-      <c r="T34" s="3" t="s">
-        <v>163</v>
+        <v>361</v>
+      </c>
+      <c r="T34" t="s">
+        <v>362</v>
       </c>
       <c r="U34">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="2">
-        <v>1</v>
-      </c>
-      <c r="C35" s="2">
-        <v>1</v>
-      </c>
-      <c r="D35" s="2"/>
+        <v>160</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2">
+        <v>1</v>
+      </c>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
-      <c r="K35" s="2">
-        <v>1</v>
-      </c>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2">
+        <v>1</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1</v>
+      </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
       <c r="P35" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="Q35" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="R35" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="S35" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="T35" s="3" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="U35">
         <v>3</v>
@@ -4089,10 +4123,14 @@
     </row>
     <row r="36" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>168</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2"/>
+        <v>164</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -4100,35 +4138,35 @@
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2">
-        <v>1</v>
-      </c>
+      <c r="K36" s="2">
+        <v>1</v>
+      </c>
+      <c r="L36" s="2"/>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
       <c r="P36" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="Q36" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="R36" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="S36" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="T36" s="3" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="U36">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -4139,27 +4177,27 @@
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-      <c r="K37" s="2">
-        <v>1</v>
-      </c>
-      <c r="L37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2">
+        <v>1</v>
+      </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
       <c r="O37" s="2"/>
       <c r="P37" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="Q37" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="R37" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="S37" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="T37" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="U37">
         <v>1</v>
@@ -4167,35 +4205,29 @@
     </row>
     <row r="38" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
+      <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="2">
-        <v>1</v>
-      </c>
+      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="2">
-        <v>1</v>
-      </c>
+      <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="2">
-        <v>1</v>
-      </c>
+      <c r="I38" s="2"/>
       <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
+      <c r="K38" s="2">
+        <v>1</v>
+      </c>
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2"/>
       <c r="P38" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="Q38" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="R38" t="s">
         <v>36</v>
@@ -4204,93 +4236,95 @@
         <v>174</v>
       </c>
       <c r="T38" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="U38">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="2"/>
+      <c r="C39" s="2">
+        <v>1</v>
+      </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2">
         <v>1</v>
       </c>
       <c r="F39" s="2"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2">
+        <v>1</v>
+      </c>
       <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
+      <c r="I39" s="2">
+        <v>1</v>
+      </c>
       <c r="J39" s="2"/>
-      <c r="K39" s="2">
-        <v>1</v>
-      </c>
-      <c r="L39" s="2">
-        <v>1</v>
-      </c>
+      <c r="K39" s="2"/>
+      <c r="L39" s="2"/>
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
-      <c r="P39" s="4" t="s">
-        <v>180</v>
+      <c r="P39" t="s">
+        <v>177</v>
       </c>
       <c r="Q39" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="R39" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S39" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="T39" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="U39">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="40" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2">
-        <v>1</v>
-      </c>
+      <c r="E40" s="2">
+        <v>1</v>
+      </c>
+      <c r="F40" s="2"/>
       <c r="G40" s="2"/>
-      <c r="H40" s="2">
-        <v>1</v>
-      </c>
+      <c r="H40" s="2"/>
       <c r="I40" s="2"/>
       <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
+      <c r="K40" s="2">
+        <v>1</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1</v>
+      </c>
       <c r="M40" s="2"/>
-      <c r="N40" s="2">
-        <v>1</v>
-      </c>
+      <c r="N40" s="2"/>
       <c r="O40" s="2"/>
-      <c r="P40" t="s">
-        <v>184</v>
+      <c r="P40" s="4" t="s">
+        <v>180</v>
       </c>
       <c r="Q40" t="s">
-        <v>185</v>
+        <v>66</v>
       </c>
       <c r="R40" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="S40" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="T40" s="3" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="U40">
         <v>3</v>
@@ -4298,20 +4332,20 @@
     </row>
     <row r="41" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
+      <c r="F41" s="2">
+        <v>1</v>
+      </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2">
         <v>1</v>
       </c>
-      <c r="I41" s="2">
-        <v>1</v>
-      </c>
+      <c r="I41" s="2"/>
       <c r="J41" s="2"/>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -4321,19 +4355,19 @@
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="Q41" t="s">
-        <v>29</v>
+        <v>185</v>
       </c>
       <c r="R41" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="S41" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="T41" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="U41">
         <v>3</v>
@@ -4341,7 +4375,7 @@
     </row>
     <row r="42" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -4349,48 +4383,46 @@
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
+      <c r="H42" s="2">
+        <v>1</v>
+      </c>
+      <c r="I42" s="2">
+        <v>1</v>
+      </c>
       <c r="J42" s="2"/>
       <c r="K42" s="2"/>
-      <c r="L42" s="2">
-        <v>1</v>
-      </c>
-      <c r="M42" s="2">
-        <v>1</v>
-      </c>
-      <c r="N42" s="2"/>
+      <c r="L42" s="2"/>
+      <c r="M42" s="2"/>
+      <c r="N42" s="2">
+        <v>1</v>
+      </c>
       <c r="O42" s="2"/>
       <c r="P42" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="Q42" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="R42" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="S42" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="T42" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="U42">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>196</v>
-      </c>
-      <c r="B43" s="2">
-        <v>1</v>
-      </c>
+        <v>192</v>
+      </c>
+      <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="2">
-        <v>1</v>
-      </c>
+      <c r="D43" s="2"/>
       <c r="E43" s="2"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -4398,218 +4430,222 @@
       <c r="I43" s="2"/>
       <c r="J43" s="2"/>
       <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2">
-        <v>1</v>
-      </c>
+      <c r="L43" s="2">
+        <v>1</v>
+      </c>
+      <c r="M43" s="2">
+        <v>1</v>
+      </c>
+      <c r="N43" s="2"/>
       <c r="O43" s="2"/>
       <c r="P43" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Q43" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="R43" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S43" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="T43" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="U43">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>200</v>
-      </c>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2">
-        <v>1</v>
-      </c>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2">
-        <v>1</v>
-      </c>
+        <v>196</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2">
+        <v>1</v>
+      </c>
+      <c r="E44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
-      <c r="H44" s="2">
-        <v>1</v>
-      </c>
-      <c r="I44" s="2">
-        <v>1</v>
-      </c>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
       <c r="J44" s="2"/>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
       <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
+      <c r="N44" s="2">
+        <v>1</v>
+      </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="Q44" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="R44" t="s">
         <v>42</v>
       </c>
       <c r="S44" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="T44" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="U44">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B45" s="2"/>
-      <c r="C45" s="2"/>
+      <c r="C45" s="2">
+        <v>1</v>
+      </c>
       <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="E45" s="2">
+        <v>1</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2">
-        <v>1</v>
-      </c>
-      <c r="K45" s="2">
-        <v>1</v>
-      </c>
+      <c r="H45" s="2">
+        <v>1</v>
+      </c>
+      <c r="I45" s="2">
+        <v>1</v>
+      </c>
+      <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
       <c r="P45" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="Q45" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R45" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="S45" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="T45" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="U45">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>208</v>
-      </c>
-      <c r="B46" s="2">
-        <v>1</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="2">
-        <v>1</v>
-      </c>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2">
-        <v>1</v>
-      </c>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2">
+        <v>1</v>
+      </c>
+      <c r="K46" s="2">
+        <v>1</v>
+      </c>
+      <c r="L46" s="2"/>
       <c r="M46" s="2"/>
-      <c r="N46" s="2">
-        <v>1</v>
-      </c>
+      <c r="N46" s="2"/>
       <c r="O46" s="2"/>
       <c r="P46" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="Q46" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="R46" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="S46" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="T46" s="3" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="U46">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>212</v>
-      </c>
-      <c r="B47" s="2"/>
+        <v>208</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1</v>
+      </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="2">
-        <v>1</v>
-      </c>
+      <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="H47" s="2">
-        <v>1</v>
-      </c>
+      <c r="H47" s="2"/>
       <c r="I47" s="2">
         <v>1</v>
       </c>
       <c r="J47" s="2"/>
       <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="L47" s="2">
+        <v>1</v>
+      </c>
       <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
+      <c r="N47" s="2">
+        <v>1</v>
+      </c>
       <c r="O47" s="2"/>
       <c r="P47" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="Q47" t="s">
-        <v>29</v>
+        <v>56</v>
       </c>
       <c r="R47" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="S47" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="T47" s="3" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="U47">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="2">
-        <v>1</v>
-      </c>
-      <c r="H48" s="2"/>
+      <c r="F48" s="2">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2"/>
+      <c r="H48" s="2">
+        <v>1</v>
+      </c>
       <c r="I48" s="2">
         <v>1</v>
       </c>
@@ -4617,46 +4653,40 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="2">
-        <v>1</v>
-      </c>
-      <c r="O48" s="2">
-        <v>1</v>
-      </c>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
       <c r="P48" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="Q48" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="R48" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="S48" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="T48" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="U48">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
-      <c r="D49" s="2">
-        <v>1</v>
-      </c>
+      <c r="D49" s="2"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2">
-        <v>1</v>
-      </c>
+      <c r="G49" s="2">
+        <v>1</v>
+      </c>
+      <c r="H49" s="2"/>
       <c r="I49" s="2">
         <v>1</v>
       </c>
@@ -4667,21 +4697,23 @@
       <c r="N49" s="2">
         <v>1</v>
       </c>
-      <c r="O49" s="2"/>
+      <c r="O49" s="2">
+        <v>1</v>
+      </c>
       <c r="P49" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="Q49" t="s">
-        <v>23</v>
+        <v>56</v>
       </c>
       <c r="R49" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="S49" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="T49" s="3" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="U49">
         <v>4</v>
@@ -4689,138 +4721,144 @@
     </row>
     <row r="50" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
+      <c r="D50" s="2">
+        <v>1</v>
+      </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
+      <c r="H50" s="2">
+        <v>1</v>
+      </c>
+      <c r="I50" s="2">
+        <v>1</v>
+      </c>
       <c r="J50" s="2"/>
-      <c r="K50" s="2">
-        <v>1</v>
-      </c>
-      <c r="L50" s="2">
-        <v>1</v>
-      </c>
+      <c r="K50" s="2"/>
+      <c r="L50" s="2"/>
       <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+      <c r="N50" s="2">
+        <v>1</v>
+      </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="Q50" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="R50" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="S50" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="T50" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="U50">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B51" s="2"/>
-      <c r="C51" s="2">
-        <v>1</v>
-      </c>
+      <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="2">
-        <v>1</v>
-      </c>
+      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="H51" s="2">
-        <v>1</v>
-      </c>
-      <c r="I51" s="2">
-        <v>1</v>
-      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2"/>
       <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
+      <c r="K51" s="2">
+        <v>1</v>
+      </c>
+      <c r="L51" s="2">
+        <v>1</v>
+      </c>
       <c r="M51" s="2"/>
-      <c r="N51" s="2">
-        <v>1</v>
-      </c>
+      <c r="N51" s="2"/>
       <c r="O51" s="2"/>
       <c r="P51" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="Q51" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="R51" t="s">
         <v>36</v>
       </c>
       <c r="S51" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="T51" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="U51">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>232</v>
-      </c>
-      <c r="B52" s="2">
-        <v>1</v>
-      </c>
-      <c r="C52" s="2"/>
+        <v>228</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2">
+        <v>1</v>
+      </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
+      <c r="F52" s="2">
+        <v>1</v>
+      </c>
       <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
+      <c r="H52" s="2">
+        <v>1</v>
+      </c>
+      <c r="I52" s="2">
+        <v>1</v>
+      </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
       <c r="L52" s="2"/>
       <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2">
-        <v>1</v>
-      </c>
+      <c r="N52" s="2">
+        <v>1</v>
+      </c>
+      <c r="O52" s="2"/>
       <c r="P52" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="Q52" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="R52" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S52" t="s">
         <v>230</v>
       </c>
       <c r="T52" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="U52">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>235</v>
-      </c>
-      <c r="B53" s="2"/>
+        <v>232</v>
+      </c>
+      <c r="B53" s="2">
+        <v>1</v>
+      </c>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
@@ -4828,44 +4866,38 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
-      <c r="J53" s="2">
-        <v>1</v>
-      </c>
-      <c r="K53" s="2">
-        <v>1</v>
-      </c>
-      <c r="L53" s="2">
-        <v>1</v>
-      </c>
+      <c r="J53" s="2"/>
+      <c r="K53" s="2"/>
+      <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
+      <c r="O53" s="2">
+        <v>1</v>
+      </c>
       <c r="P53" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="Q53" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="R53" t="s">
         <v>42</v>
       </c>
       <c r="S53" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="T53" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="U53">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>239</v>
-      </c>
-      <c r="B54" s="2">
-        <v>1</v>
-      </c>
+        <v>235</v>
+      </c>
+      <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
@@ -4873,30 +4905,32 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
+      <c r="J54" s="2">
+        <v>1</v>
+      </c>
       <c r="K54" s="2">
         <v>1</v>
       </c>
-      <c r="L54" s="2"/>
+      <c r="L54" s="2">
+        <v>1</v>
+      </c>
       <c r="M54" s="2"/>
       <c r="N54" s="2"/>
-      <c r="O54" s="2">
-        <v>1</v>
-      </c>
+      <c r="O54" s="2"/>
       <c r="P54" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="Q54" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="R54" t="s">
         <v>42</v>
       </c>
       <c r="S54" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="T54" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="U54">
         <v>3</v>
@@ -4904,7 +4938,7 @@
     </row>
     <row r="55" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B55" s="2">
         <v>1</v>
@@ -4912,16 +4946,14 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="2">
-        <v>1</v>
-      </c>
+      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="H55" s="2">
-        <v>1</v>
-      </c>
+      <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
+      <c r="K55" s="2">
+        <v>1</v>
+      </c>
       <c r="L55" s="2"/>
       <c r="M55" s="2"/>
       <c r="N55" s="2"/>
@@ -4929,7 +4961,7 @@
         <v>1</v>
       </c>
       <c r="P55" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="Q55" t="s">
         <v>51</v>
@@ -4938,61 +4970,63 @@
         <v>42</v>
       </c>
       <c r="S55" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="T55" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="U55">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>247</v>
-      </c>
-      <c r="B56" s="2"/>
+        <v>243</v>
+      </c>
+      <c r="B56" s="2">
+        <v>1</v>
+      </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="2"/>
+      <c r="F56" s="2">
+        <v>1</v>
+      </c>
       <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
+      <c r="H56" s="2">
+        <v>1</v>
+      </c>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
-      <c r="K56" s="2">
-        <v>1</v>
-      </c>
-      <c r="L56" s="2">
-        <v>1</v>
-      </c>
-      <c r="M56" s="2">
-        <v>1</v>
-      </c>
+      <c r="K56" s="2"/>
+      <c r="L56" s="2"/>
+      <c r="M56" s="2"/>
       <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
+      <c r="O56" s="2">
+        <v>1</v>
+      </c>
       <c r="P56" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="Q56" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="R56" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="S56" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="T56" s="3" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="U56">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="57" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -5003,44 +5037,44 @@
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
       <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
+      <c r="K57" s="2">
+        <v>1</v>
+      </c>
       <c r="L57" s="2">
         <v>1</v>
       </c>
-      <c r="M57" s="2"/>
+      <c r="M57" s="2">
+        <v>1</v>
+      </c>
       <c r="N57" s="2"/>
       <c r="O57" s="2"/>
       <c r="P57" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="Q57" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="R57" t="s">
         <v>36</v>
       </c>
       <c r="S57" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="T57" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="U57">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
-      <c r="D58" s="2">
-        <v>1</v>
-      </c>
-      <c r="E58" s="2">
-        <v>1</v>
-      </c>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -5050,39 +5084,37 @@
       <c r="L58" s="2">
         <v>1</v>
       </c>
-      <c r="M58" s="2">
-        <v>1</v>
-      </c>
-      <c r="N58" s="2">
-        <v>1</v>
-      </c>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
       <c r="O58" s="2"/>
       <c r="P58" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="Q58" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="R58" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="S58" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="T58" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="U58">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
-      <c r="D59" s="2"/>
+      <c r="D59" s="2">
+        <v>1</v>
+      </c>
       <c r="E59" s="2">
         <v>1</v>
       </c>
@@ -5092,7 +5124,9 @@
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
+      <c r="L59" s="2">
+        <v>1</v>
+      </c>
       <c r="M59" s="2">
         <v>1</v>
       </c>
@@ -5101,62 +5135,62 @@
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="Q59" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="R59" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="S59" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="T59" s="3" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="U59">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
-      <c r="D60" s="2">
-        <v>1</v>
-      </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2">
-        <v>1</v>
-      </c>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
       <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
+      <c r="M60" s="2">
+        <v>1</v>
+      </c>
       <c r="N60" s="2">
         <v>1</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="Q60" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="R60" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="S60" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="T60" s="3" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="U60">
         <v>3</v>
@@ -5164,95 +5198,95 @@
     </row>
     <row r="61" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2">
         <v>1</v>
       </c>
-      <c r="E61" s="2">
-        <v>1</v>
-      </c>
-      <c r="F61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
-      <c r="K61" s="2">
-        <v>1</v>
-      </c>
-      <c r="L61" s="2">
-        <v>1</v>
-      </c>
+      <c r="K61" s="2"/>
+      <c r="L61" s="2"/>
       <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
+      <c r="N61" s="2">
+        <v>1</v>
+      </c>
       <c r="O61" s="2"/>
       <c r="P61" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="Q61" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="R61" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="S61" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="T61" s="3" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="U61">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2"/>
+      <c r="D62" s="2">
+        <v>1</v>
+      </c>
+      <c r="E62" s="2">
+        <v>1</v>
+      </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="H62" s="2">
-        <v>1</v>
-      </c>
-      <c r="I62" s="2">
-        <v>1</v>
-      </c>
+      <c r="H62" s="2"/>
+      <c r="I62" s="2"/>
       <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
+      <c r="K62" s="2">
+        <v>1</v>
+      </c>
+      <c r="L62" s="2">
+        <v>1</v>
+      </c>
       <c r="M62" s="2"/>
-      <c r="N62" s="2">
-        <v>1</v>
-      </c>
+      <c r="N62" s="2"/>
       <c r="O62" s="2"/>
       <c r="P62" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="Q62" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="R62" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="S62" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="T62" s="3" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="U62">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -5260,105 +5294,109 @@
       <c r="E63" s="2"/>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
+      <c r="H63" s="2">
+        <v>1</v>
+      </c>
+      <c r="I63" s="2">
+        <v>1</v>
+      </c>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
-      <c r="L63" s="2">
-        <v>1</v>
-      </c>
+      <c r="L63" s="2"/>
       <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
+      <c r="N63" s="2">
+        <v>1</v>
+      </c>
       <c r="O63" s="2"/>
       <c r="P63" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="Q63" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="R63" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="S63" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="T63" s="3" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="U63">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>279</v>
-      </c>
-      <c r="B64" s="2">
-        <v>1</v>
-      </c>
-      <c r="C64" s="2">
-        <v>1</v>
-      </c>
+        <v>275</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
-      <c r="G64" s="2">
-        <v>1</v>
-      </c>
+      <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
-      <c r="J64" s="2">
-        <v>1</v>
-      </c>
+      <c r="J64" s="2"/>
       <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
+      <c r="L64" s="2">
+        <v>1</v>
+      </c>
       <c r="M64" s="2"/>
       <c r="N64" s="2"/>
       <c r="O64" s="2"/>
       <c r="P64" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="Q64" t="s">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="R64" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="S64" t="s">
-        <v>281</v>
-      </c>
-      <c r="T64" t="s">
-        <v>282</v>
+        <v>277</v>
+      </c>
+      <c r="T64" s="3" t="s">
+        <v>278</v>
       </c>
       <c r="U64">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B65" s="2">
         <v>1</v>
       </c>
-      <c r="C65" s="2"/>
+      <c r="C65" s="2">
+        <v>1</v>
+      </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
-      <c r="G65" s="2"/>
+      <c r="G65" s="2">
+        <v>1</v>
+      </c>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
+      <c r="J65" s="2">
+        <v>1</v>
+      </c>
       <c r="K65" s="2"/>
       <c r="L65" s="2"/>
       <c r="M65" s="2"/>
       <c r="N65" s="2"/>
       <c r="O65" s="2"/>
       <c r="P65" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="Q65" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
       <c r="R65" t="s">
         <v>42</v>
@@ -5366,256 +5404,250 @@
       <c r="S65" t="s">
         <v>281</v>
       </c>
-      <c r="T65" s="3" t="s">
-        <v>285</v>
+      <c r="T65" t="s">
+        <v>282</v>
       </c>
       <c r="U65">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>286</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2">
-        <v>1</v>
-      </c>
-      <c r="D66" s="2">
-        <v>1</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="B66" s="2">
+        <v>1</v>
+      </c>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
       <c r="E66" s="2"/>
       <c r="F66" s="2"/>
-      <c r="G66" s="2">
-        <v>1</v>
-      </c>
+      <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
-      <c r="J66" s="2">
-        <v>1</v>
-      </c>
+      <c r="J66" s="2"/>
       <c r="K66" s="2"/>
       <c r="L66" s="2"/>
       <c r="M66" s="2"/>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
       <c r="P66" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="Q66" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="R66" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="S66" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="T66" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="U66">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>290</v>
-      </c>
-      <c r="B67" s="2">
-        <v>1</v>
-      </c>
-      <c r="C67" s="2"/>
-      <c r="D67" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="2">
+        <v>1</v>
+      </c>
+      <c r="D67" s="2">
+        <v>1</v>
+      </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
+      <c r="G67" s="2">
+        <v>1</v>
+      </c>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2">
         <v>1</v>
       </c>
-      <c r="K67" s="2">
-        <v>1</v>
-      </c>
+      <c r="K67" s="2"/>
       <c r="L67" s="2"/>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
       <c r="O67" s="2"/>
       <c r="P67" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="Q67" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="R67" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="S67" t="s">
-        <v>292</v>
-      </c>
-      <c r="T67" t="s">
-        <v>293</v>
+        <v>288</v>
+      </c>
+      <c r="T67" s="3" t="s">
+        <v>289</v>
       </c>
       <c r="U67">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>294</v>
-      </c>
-      <c r="B68" s="2"/>
+        <v>290</v>
+      </c>
+      <c r="B68" s="2">
+        <v>1</v>
+      </c>
       <c r="C68" s="2"/>
-      <c r="D68" s="2">
-        <v>1</v>
-      </c>
+      <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="F68" s="2">
-        <v>1</v>
-      </c>
+      <c r="F68" s="2"/>
       <c r="G68" s="2"/>
-      <c r="H68" s="2">
-        <v>1</v>
-      </c>
+      <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
+      <c r="J68" s="2">
+        <v>1</v>
+      </c>
+      <c r="K68" s="2">
+        <v>1</v>
+      </c>
       <c r="L68" s="2"/>
-      <c r="M68" s="2">
-        <v>1</v>
-      </c>
-      <c r="N68" s="2">
-        <v>1</v>
-      </c>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
       <c r="O68" s="2"/>
       <c r="P68" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="Q68" t="s">
-        <v>185</v>
+        <v>56</v>
       </c>
       <c r="R68" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="S68" t="s">
-        <v>296</v>
-      </c>
-      <c r="T68" s="3" t="s">
-        <v>297</v>
+        <v>292</v>
+      </c>
+      <c r="T68" t="s">
+        <v>293</v>
       </c>
       <c r="U68">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
+      <c r="D69" s="2">
+        <v>1</v>
+      </c>
       <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
+      <c r="F69" s="2">
+        <v>1</v>
+      </c>
       <c r="G69" s="2"/>
-      <c r="H69" s="2"/>
+      <c r="H69" s="2">
+        <v>1</v>
+      </c>
       <c r="I69" s="2"/>
       <c r="J69" s="2"/>
       <c r="K69" s="2"/>
       <c r="L69" s="2"/>
-      <c r="M69" s="2"/>
-      <c r="N69" s="2"/>
-      <c r="O69" s="2">
-        <v>1</v>
-      </c>
+      <c r="M69" s="2">
+        <v>1</v>
+      </c>
+      <c r="N69" s="2">
+        <v>1</v>
+      </c>
+      <c r="O69" s="2"/>
       <c r="P69" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="Q69" t="s">
-        <v>51</v>
+        <v>185</v>
       </c>
       <c r="R69" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="S69" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="T69" s="3" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="U69">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B70" s="2"/>
-      <c r="C70" s="2">
-        <v>1</v>
-      </c>
+      <c r="C70" s="2"/>
       <c r="D70" s="2"/>
-      <c r="E70" s="2">
-        <v>1</v>
-      </c>
+      <c r="E70" s="2"/>
       <c r="F70" s="2"/>
-      <c r="G70" s="2">
-        <v>1</v>
-      </c>
+      <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
-      <c r="J70" s="2">
-        <v>1</v>
-      </c>
-      <c r="K70" s="2">
-        <v>1</v>
-      </c>
+      <c r="J70" s="2"/>
+      <c r="K70" s="2"/>
       <c r="L70" s="2"/>
       <c r="M70" s="2"/>
-      <c r="N70" s="2">
-        <v>1</v>
-      </c>
-      <c r="O70" s="2"/>
+      <c r="N70" s="2"/>
+      <c r="O70" s="2">
+        <v>1</v>
+      </c>
       <c r="P70" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="Q70" t="s">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="R70" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="S70" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="T70" s="3" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="U70">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B71" s="2"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="2">
-        <v>1</v>
-      </c>
-      <c r="E71" s="2"/>
+      <c r="C71" s="2">
+        <v>1</v>
+      </c>
+      <c r="D71" s="2"/>
+      <c r="E71" s="2">
+        <v>1</v>
+      </c>
       <c r="F71" s="2"/>
-      <c r="G71" s="2"/>
-      <c r="H71" s="2">
-        <v>1</v>
-      </c>
-      <c r="I71" s="2">
-        <v>1</v>
-      </c>
-      <c r="J71" s="2"/>
-      <c r="K71" s="2"/>
+      <c r="G71" s="2">
+        <v>1</v>
+      </c>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2"/>
+      <c r="J71" s="2">
+        <v>1</v>
+      </c>
+      <c r="K71" s="2">
+        <v>1</v>
+      </c>
       <c r="L71" s="2"/>
       <c r="M71" s="2"/>
       <c r="N71" s="2">
@@ -5623,31 +5655,33 @@
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="Q71" t="s">
-        <v>35</v>
+        <v>185</v>
       </c>
       <c r="R71" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="S71" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="T71" s="3" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="U71">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="72" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="D72" s="2">
+        <v>1</v>
+      </c>
       <c r="E72" s="2"/>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -5666,72 +5700,70 @@
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="Q72" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="R72" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="S72" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="T72" s="3" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="U72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>314</v>
-      </c>
-      <c r="B73" s="2">
-        <v>1</v>
-      </c>
+        <v>310</v>
+      </c>
+      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
-      <c r="G73" s="2">
-        <v>1</v>
-      </c>
-      <c r="H73" s="2"/>
-      <c r="I73" s="2"/>
-      <c r="J73" s="2">
-        <v>1</v>
-      </c>
-      <c r="K73" s="2">
-        <v>1</v>
-      </c>
+      <c r="G73" s="2"/>
+      <c r="H73" s="2">
+        <v>1</v>
+      </c>
+      <c r="I73" s="2">
+        <v>1</v>
+      </c>
+      <c r="J73" s="2"/>
+      <c r="K73" s="2"/>
       <c r="L73" s="2"/>
       <c r="M73" s="2"/>
-      <c r="N73" s="2"/>
+      <c r="N73" s="2">
+        <v>1</v>
+      </c>
       <c r="O73" s="2"/>
       <c r="P73" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="Q73" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="R73" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="S73" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="T73" s="3" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="U73">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="74" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="B74" s="2">
         <v>1</v>
@@ -5740,176 +5772,176 @@
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
-      <c r="G74" s="2"/>
+      <c r="G74" s="2">
+        <v>1</v>
+      </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
-      <c r="J74" s="2"/>
-      <c r="K74" s="2"/>
+      <c r="J74" s="2">
+        <v>1</v>
+      </c>
+      <c r="K74" s="2">
+        <v>1</v>
+      </c>
       <c r="L74" s="2"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
-      <c r="P74" s="4" t="s">
-        <v>319</v>
+      <c r="P74" t="s">
+        <v>315</v>
       </c>
       <c r="Q74" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="R74" t="s">
         <v>42</v>
       </c>
       <c r="S74" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="T74" s="3" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="U74">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="75" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="B75" s="2">
         <v>1</v>
       </c>
-      <c r="C75" s="2">
-        <v>1</v>
-      </c>
+      <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
-      <c r="J75" s="2">
-        <v>1</v>
-      </c>
+      <c r="J75" s="2"/>
       <c r="K75" s="2"/>
       <c r="L75" s="2"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
-      <c r="P75" t="s">
-        <v>323</v>
+      <c r="P75" s="4" t="s">
+        <v>319</v>
       </c>
       <c r="Q75" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="R75" t="s">
         <v>42</v>
       </c>
       <c r="S75" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="T75" s="3" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="U75">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>326</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2">
-        <v>1</v>
-      </c>
-      <c r="E76" s="2">
-        <v>1</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="B76" s="2">
+        <v>1</v>
+      </c>
+      <c r="C76" s="2">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
-      <c r="J76" s="2"/>
+      <c r="J76" s="2">
+        <v>1</v>
+      </c>
       <c r="K76" s="2"/>
       <c r="L76" s="2"/>
-      <c r="M76" s="2">
-        <v>1</v>
-      </c>
-      <c r="N76" s="2">
-        <v>1</v>
-      </c>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
       <c r="O76" s="2"/>
       <c r="P76" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="Q76" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="R76" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="S76" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="T76" s="3" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="U76">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2">
         <v>1</v>
       </c>
-      <c r="E77" s="2"/>
-      <c r="F77" s="2">
-        <v>1</v>
-      </c>
-      <c r="G77" s="2">
-        <v>1</v>
-      </c>
+      <c r="E77" s="2">
+        <v>1</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
       <c r="H77" s="2"/>
-      <c r="I77" s="2">
-        <v>1</v>
-      </c>
+      <c r="I77" s="2"/>
       <c r="J77" s="2"/>
       <c r="K77" s="2"/>
       <c r="L77" s="2"/>
       <c r="M77" s="2">
         <v>1</v>
       </c>
-      <c r="N77" s="2"/>
+      <c r="N77" s="2">
+        <v>1</v>
+      </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="Q77" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="R77" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="S77" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="T77" s="3" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="U77">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2">
+        <v>1</v>
+      </c>
       <c r="E78" s="2"/>
       <c r="F78" s="2">
         <v>1</v>
@@ -5923,28 +5955,26 @@
       </c>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
-      <c r="L78" s="2">
-        <v>1</v>
-      </c>
-      <c r="M78" s="2"/>
-      <c r="N78" s="2">
-        <v>1</v>
-      </c>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2">
+        <v>1</v>
+      </c>
+      <c r="N78" s="2"/>
       <c r="O78" s="2"/>
       <c r="P78" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="Q78" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="R78" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="S78" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="T78" s="3" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="U78">
         <v>5</v>
@@ -5952,85 +5982,89 @@
     </row>
     <row r="79" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>338</v>
-      </c>
-      <c r="B79" s="2">
-        <v>1</v>
-      </c>
+        <v>334</v>
+      </c>
+      <c r="B79" s="2"/>
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
-      <c r="F79" s="2"/>
-      <c r="G79" s="2"/>
+      <c r="F79" s="2">
+        <v>1</v>
+      </c>
+      <c r="G79" s="2">
+        <v>1</v>
+      </c>
       <c r="H79" s="2"/>
-      <c r="I79" s="2"/>
+      <c r="I79" s="2">
+        <v>1</v>
+      </c>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
       <c r="L79" s="2">
         <v>1</v>
       </c>
-      <c r="M79" s="2">
-        <v>1</v>
-      </c>
-      <c r="N79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2">
+        <v>1</v>
+      </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="Q79" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="R79" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="S79" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="T79" s="3" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="U79">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>342</v>
-      </c>
-      <c r="B80" s="2"/>
+        <v>338</v>
+      </c>
+      <c r="B80" s="2">
+        <v>1</v>
+      </c>
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
-      <c r="H80" s="2">
-        <v>1</v>
-      </c>
-      <c r="I80" s="2">
-        <v>1</v>
-      </c>
-      <c r="J80" s="2">
-        <v>1</v>
-      </c>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
       <c r="K80" s="2"/>
-      <c r="L80" s="2"/>
-      <c r="M80" s="2"/>
+      <c r="L80" s="2">
+        <v>1</v>
+      </c>
+      <c r="M80" s="2">
+        <v>1</v>
+      </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
       <c r="P80" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="Q80" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="R80" t="s">
         <v>36</v>
       </c>
       <c r="S80" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="T80" s="3" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="U80">
         <v>3</v>
@@ -6038,42 +6072,42 @@
     </row>
     <row r="81" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="B81" s="2"/>
-      <c r="C81" s="2">
-        <v>1</v>
-      </c>
+      <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
-      <c r="H81" s="2"/>
-      <c r="I81" s="2"/>
+      <c r="H81" s="2">
+        <v>1</v>
+      </c>
+      <c r="I81" s="2">
+        <v>1</v>
+      </c>
       <c r="J81" s="2">
         <v>1</v>
       </c>
-      <c r="K81" s="2">
-        <v>1</v>
-      </c>
+      <c r="K81" s="2"/>
       <c r="L81" s="2"/>
       <c r="M81" s="2"/>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
       <c r="P81" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="Q81" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
       <c r="R81" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
       <c r="S81" t="s">
         <v>344</v>
       </c>
       <c r="T81" s="3" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="U81">
         <v>3</v>
@@ -6081,74 +6115,72 @@
     </row>
     <row r="82" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>349</v>
-      </c>
-      <c r="B82" s="2">
-        <v>1</v>
-      </c>
-      <c r="C82" s="2"/>
+        <v>346</v>
+      </c>
+      <c r="B82" s="2"/>
+      <c r="C82" s="2">
+        <v>1</v>
+      </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
-      <c r="J82" s="2"/>
-      <c r="K82" s="2"/>
+      <c r="J82" s="2">
+        <v>1</v>
+      </c>
+      <c r="K82" s="2">
+        <v>1</v>
+      </c>
       <c r="L82" s="2"/>
       <c r="M82" s="2"/>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
       <c r="P82" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="Q82" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="R82" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="S82" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="T82" s="3" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="U82">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>353</v>
-      </c>
-      <c r="B83" s="2"/>
+        <v>349</v>
+      </c>
+      <c r="B83" s="2">
+        <v>1</v>
+      </c>
       <c r="C83" s="2"/>
-      <c r="D83" s="2">
-        <v>1</v>
-      </c>
+      <c r="D83" s="2"/>
       <c r="E83" s="2"/>
-      <c r="F83" s="2">
-        <v>1</v>
-      </c>
+      <c r="F83" s="2"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
-      <c r="J83" s="2">
-        <v>1</v>
-      </c>
+      <c r="J83" s="2"/>
       <c r="K83" s="2"/>
       <c r="L83" s="2"/>
-      <c r="M83" s="2">
-        <v>1</v>
-      </c>
+      <c r="M83" s="2"/>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
       <c r="P83" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="Q83" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="R83" t="s">
         <v>42</v>
@@ -6157,48 +6189,93 @@
         <v>351</v>
       </c>
       <c r="T83" s="3" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="U83">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2">
+        <v>1</v>
+      </c>
       <c r="E84" s="2"/>
-      <c r="F84" s="2"/>
+      <c r="F84" s="2">
+        <v>1</v>
+      </c>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
-      <c r="J84" s="2"/>
+      <c r="J84" s="2">
+        <v>1</v>
+      </c>
       <c r="K84" s="2"/>
-      <c r="L84" s="2">
-        <v>1</v>
-      </c>
-      <c r="M84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2">
+        <v>1</v>
+      </c>
       <c r="N84" s="2"/>
       <c r="O84" s="2"/>
       <c r="P84" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="Q84" t="s">
-        <v>23</v>
+        <v>51</v>
       </c>
       <c r="R84" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="S84" t="s">
         <v>351</v>
       </c>
       <c r="T84" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="U84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:21" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>356</v>
+      </c>
+      <c r="B85" s="2"/>
+      <c r="C85" s="2"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="2"/>
+      <c r="F85" s="2"/>
+      <c r="G85" s="2"/>
+      <c r="H85" s="2"/>
+      <c r="I85" s="2"/>
+      <c r="J85" s="2"/>
+      <c r="K85" s="2"/>
+      <c r="L85" s="2">
+        <v>1</v>
+      </c>
+      <c r="M85" s="2"/>
+      <c r="N85" s="2"/>
+      <c r="O85" s="2"/>
+      <c r="P85" t="s">
+        <v>357</v>
+      </c>
+      <c r="Q85" t="s">
+        <v>23</v>
+      </c>
+      <c r="R85" t="s">
+        <v>24</v>
+      </c>
+      <c r="S85" t="s">
+        <v>351</v>
+      </c>
+      <c r="T85" s="3" t="s">
         <v>358</v>
       </c>
-      <c r="U84">
+      <c r="U85">
         <v>1</v>
       </c>
     </row>
@@ -6208,8 +6285,8 @@
     <hyperlink ref="P15" r:id="rId2" xr:uid="{1A3073E5-A6C0-4F06-AB44-1FDB7CB13897}"/>
     <hyperlink ref="P25" r:id="rId3" xr:uid="{A485F6D0-3B9E-4335-9DEB-9EC9B463480A}"/>
     <hyperlink ref="P29" r:id="rId4" xr:uid="{08AF599A-2895-43FF-ADB1-E19995DA280A}"/>
-    <hyperlink ref="P39" r:id="rId5" xr:uid="{24AB1B4F-999C-4EFE-A755-DC8FAAB642B1}"/>
-    <hyperlink ref="P74" r:id="rId6" xr:uid="{EDB78E41-2F1C-48C2-AF32-85DF1C542435}"/>
+    <hyperlink ref="P40" r:id="rId5" xr:uid="{24AB1B4F-999C-4EFE-A755-DC8FAAB642B1}"/>
+    <hyperlink ref="P75" r:id="rId6" xr:uid="{EDB78E41-2F1C-48C2-AF32-85DF1C542435}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>